<commit_message>
Deploy til rot: LMDI - d6712f602f7ff3b72a63c349794b7697cf0e03b0
</commit_message>
<xml_diff>
--- a/StructureDefinition-lmdi-medication.xlsx
+++ b/StructureDefinition-lmdi-medication.xlsx
@@ -10025,7 +10025,7 @@
       </c>
       <c r="E74" s="2"/>
       <c r="F74" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G74" t="s" s="2">
         <v>87</v>
@@ -10943,7 +10943,7 @@
       </c>
       <c r="E82" s="2"/>
       <c r="F82" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G82" t="s" s="2">
         <v>87</v>
@@ -11173,7 +11173,7 @@
       </c>
       <c r="E84" s="2"/>
       <c r="F84" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G84" t="s" s="2">
         <v>87</v>
@@ -11293,7 +11293,7 @@
         <v>87</v>
       </c>
       <c r="H85" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="I85" t="s" s="2">
         <v>77</v>

</xml_diff>